<commit_message>
Exercícios - SCRIPTs DQL - JOIN
</commit_message>
<xml_diff>
--- a/exercicios/1.2-exercicio-locadora/Modelagem/Exercicio1.2-Locadora-FÍSICO.xlsx
+++ b/exercicios/1.2-exercicio-locadora/Modelagem/Exercicio1.2-Locadora-FÍSICO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/Banco-de-Dados/exercicios/1.2-exercicio-locadora/Modelagem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA245787-980B-4EEF-B897-AA00B5B810F1}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5176C3C-98B3-4768-8D05-D5CFDB43D341}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Empresa</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>IdAluguel</t>
-  </si>
-  <si>
-    <t>Carro</t>
   </si>
   <si>
     <t>DataAluguel</t>
@@ -434,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,10 +560,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -858,15 +851,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1132,13 +1125,7 @@
         <v>31</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1159,13 +1146,7 @@
       <c r="H12" s="56">
         <v>2</v>
       </c>
-      <c r="I12" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="64">
+      <c r="I12" s="60">
         <v>44242</v>
       </c>
     </row>
@@ -1187,13 +1168,7 @@
       <c r="H13" s="57">
         <v>3</v>
       </c>
-      <c r="I13" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="64">
+      <c r="I13" s="60">
         <v>44346</v>
       </c>
     </row>
@@ -1215,13 +1190,7 @@
       <c r="H14" s="58">
         <v>1</v>
       </c>
-      <c r="I14" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="64">
+      <c r="I14" s="60">
         <v>44400</v>
       </c>
     </row>
@@ -1235,13 +1204,7 @@
       <c r="H15" s="59">
         <v>2</v>
       </c>
-      <c r="I15" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="65">
+      <c r="I15" s="61">
         <v>44410</v>
       </c>
     </row>

</xml_diff>